<commit_message>
Update version 1.7.0 PREVIEW
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/ClientsDataExcel.xlsx
+++ b/src/test/resources/testdata/ClientsDataExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PERSONAL_PROJECT_AUTO_TEST\AutomationFrameworkSelenium\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{039E8164-0C16-41A7-AF65-C3C0E8C0B008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD8CB76-01D0-4716-8AC6-8B9A03A74E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{7A35AAC3-973C-4AA0-816A-DECEFD0ED1D8}"/>
   </bookViews>
@@ -151,13 +151,13 @@
     <t>Anh Tester</t>
   </si>
   <si>
-    <t>Anh Tester Client 0607A1</t>
-  </si>
-  <si>
-    <t>Anh Tester Client 0607A2</t>
-  </si>
-  <si>
-    <t>Anh Tester Client 0607A3</t>
+    <t>Anh Tester Client 2607A1</t>
+  </si>
+  <si>
+    <t>Anh Tester Client 2607A2</t>
+  </si>
+  <si>
+    <t>Anh Tester Client 2607A3</t>
   </si>
 </sst>
 </file>
@@ -295,15 +295,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -312,19 +312,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -659,99 +653,99 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.21875" style="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="36.21875" style="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="33.33203125" style="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.5546875" style="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.44140625" style="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.33203125" style="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="8.88671875" style="12" collapsed="1"/>
+    <col min="1" max="1" width="20.21875" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="36.21875" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="33.33203125" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.5546875" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.44140625" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.33203125" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="8.88671875" style="10" collapsed="1"/>
     <col min="9" max="16384" width="8.88671875" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="9" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -789,44 +783,44 @@
     <col min="14" max="16384" width="18.21875" style="2" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:13" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -858,7 +852,7 @@
       <c r="I2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="8" t="s">
         <v>11</v>
       </c>
       <c r="K2" s="3" t="s">
@@ -867,7 +861,6 @@
       <c r="L2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="M2" s="6"/>
     </row>
     <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -897,7 +890,7 @@
       <c r="I3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="8" t="s">
         <v>11</v>
       </c>
       <c r="K3" s="3">
@@ -906,7 +899,6 @@
       <c r="L3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="M3" s="6"/>
     </row>
     <row r="4" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
@@ -945,7 +937,6 @@
       <c r="L4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="M4" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
Update new version 1.8.0 PREVIEW
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/ClientsDataExcel.xlsx
+++ b/src/test/resources/testdata/ClientsDataExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PERSONAL_PROJECT_AUTO_TEST\AutomationFrameworkSelenium\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28BCCD02-365E-4EF2-8821-A1DEAC265FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78044C1B-7A52-43FF-8F95-FDA5DBC034EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2964" yWindow="1488" windowWidth="18600" windowHeight="10224" activeTab="1" xr2:uid="{7A35AAC3-973C-4AA0-816A-DECEFD0ED1D8}"/>
+    <workbookView xWindow="3312" yWindow="1836" windowWidth="18600" windowHeight="10224" activeTab="1" xr2:uid="{7A35AAC3-973C-4AA0-816A-DECEFD0ED1D8}"/>
   </bookViews>
   <sheets>
     <sheet name="SignIn" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
   <si>
     <t>Dong Thap</t>
   </si>
@@ -49,9 +49,6 @@
     <t>O Mon</t>
   </si>
   <si>
-    <t>T+wyT5u9cOelDJbBWNgxLw==</t>
-  </si>
-  <si>
     <t>VAT</t>
   </si>
   <si>
@@ -124,27 +121,12 @@
     <t>Thai Thi Hanh</t>
   </si>
   <si>
-    <t>admin@mailinator.com</t>
-  </si>
-  <si>
-    <t>Project Manager</t>
-  </si>
-  <si>
-    <t>projectmanager@mailinator.com</t>
-  </si>
-  <si>
     <t>testSignInData</t>
   </si>
   <si>
     <t>VIP</t>
   </si>
   <si>
-    <t>PRO</t>
-  </si>
-  <si>
-    <t>Anh Tester</t>
-  </si>
-  <si>
     <t>Anh Tester Client 1108A1</t>
   </si>
   <si>
@@ -152,15 +134,44 @@
   </si>
   <si>
     <t>Anh Tester Client 1108A3</t>
+  </si>
+  <si>
+    <t>admin@demo.com</t>
+  </si>
+  <si>
+    <t>dw5AQDhu9+WsEsWisMJISA==</t>
+  </si>
+  <si>
+    <t>client@demo.com</t>
+  </si>
+  <si>
+    <t>Gold</t>
+  </si>
+  <si>
+    <t>Mark Thomas</t>
+  </si>
+  <si>
+    <t>Richard Gray</t>
+  </si>
+  <si>
+    <t>Sara Ann</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -287,42 +298,45 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -639,17 +653,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FF288A0-DB40-4E38-9AAF-ADDED2880E84}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20.21875" style="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="36.21875" style="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="33.33203125" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.88671875" style="10" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="38" style="10" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="18.5546875" style="10" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="20.44140625" style="10" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="17.33203125" style="10" bestFit="1" customWidth="1" collapsed="1"/>
@@ -659,36 +673,36 @@
   <sheetData>
     <row r="1" spans="1:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>27</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
@@ -697,49 +711,19 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>7</v>
+        <v>31</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -756,15 +740,15 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.21875" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.88671875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="27.6640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.5546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.44140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.88671875" style="2" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="10.44140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="12.109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="9" style="2" bestFit="1" customWidth="1" collapsed="1"/>
@@ -779,54 +763,54 @@
   <sheetData>
     <row r="1" spans="1:13" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="D1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>4</v>
@@ -847,27 +831,27 @@
         <v>3</v>
       </c>
       <c r="J2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="L2" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>6</v>
@@ -885,24 +869,24 @@
         <v>3</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K3" s="3">
         <v>30</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>6</v>
@@ -923,17 +907,17 @@
         <v>3</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="J2" r:id="rId1" xr:uid="{ED197778-D3E0-411D-9BE8-9D641596BB30}"/>
     <hyperlink ref="J3" r:id="rId2" xr:uid="{6BB180CC-F100-4639-BD3A-B7B33CC640F9}"/>

</xml_diff>

<commit_message>
Update version 1.9.3 PREVIEW
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/ClientsDataExcel.xlsx
+++ b/src/test/resources/testdata/ClientsDataExcel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PERSONAL_PROJECT_AUTO_TEST\AutomationFrameworkSelenium\src\test\resources\testdata\"/>
     </mc:Choice>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
   <si>
     <t>Dong Thap</t>
   </si>
@@ -161,6 +161,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -268,7 +269,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -286,6 +287,11 @@
         <fgColor indexed="11"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="11"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -300,7 +306,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -337,6 +343,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -661,14 +670,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.21875" style="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.88671875" style="10" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="38" style="10" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.5546875" style="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.44140625" style="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.33203125" style="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="8.88671875" style="10" collapsed="1"/>
-    <col min="9" max="16384" width="8.88671875" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="10" width="20.21875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="10" width="32.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="10" width="38.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="10" width="18.5546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="10" width="20.44140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="10" width="17.33203125" collapsed="true"/>
+    <col min="7" max="8" style="10" width="8.88671875" collapsed="true"/>
+    <col min="9" max="16384" style="1" width="8.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
@@ -701,7 +710,7 @@
       <c r="C2" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="15" t="s">
         <v>28</v>
       </c>
       <c r="E2" s="11"/>
@@ -745,20 +754,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.21875" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.6640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.44140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.88671875" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.44140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.5546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.44140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="24.5546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="4.77734375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.44140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="8" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="16384" width="18.21875" style="2" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="15.88671875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="27.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="21.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="21.88671875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="10.44140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="12.109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="9.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="10.5546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="14.44140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="24.5546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="4.77734375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="15.44140625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="8.0" collapsed="true"/>
+    <col min="14" max="16384" style="2" width="18.21875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update version 1.9.4 PREVIEW
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/ClientsDataExcel.xlsx
+++ b/src/test/resources/testdata/ClientsDataExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PERSONAL_PROJECT_AUTO_TEST\AutomationFrameworkSelenium\src\test\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECT_FRAMEWORK\AutomationFrameworkSelenium\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78044C1B-7A52-43FF-8F95-FDA5DBC034EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DABB09B-FBB6-4D5A-81D5-6B1EECAD6213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3312" yWindow="1836" windowWidth="18600" windowHeight="10224" activeTab="1" xr2:uid="{7A35AAC3-973C-4AA0-816A-DECEFD0ED1D8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{7A35AAC3-973C-4AA0-816A-DECEFD0ED1D8}"/>
   </bookViews>
   <sheets>
     <sheet name="SignIn" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
   <si>
     <t>Dong Thap</t>
   </si>
@@ -112,9 +112,6 @@
     <t>EXPECTED_URL</t>
   </si>
   <si>
-    <t>pass</t>
-  </si>
-  <si>
     <t>testAddClient</t>
   </si>
   <si>
@@ -127,15 +124,6 @@
     <t>VIP</t>
   </si>
   <si>
-    <t>Anh Tester Client 1108A1</t>
-  </si>
-  <si>
-    <t>Anh Tester Client 1108A2</t>
-  </si>
-  <si>
-    <t>Anh Tester Client 1108A3</t>
-  </si>
-  <si>
     <t>admin@demo.com</t>
   </si>
   <si>
@@ -155,18 +143,26 @@
   </si>
   <si>
     <t>Sara Ann</t>
+  </si>
+  <si>
+    <t>Anh Tester Client 0403A1</t>
+  </si>
+  <si>
+    <t>Anh Tester Client 0403A2</t>
+  </si>
+  <si>
+    <t>Anh Tester Client 0403A3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -174,7 +170,7 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -182,7 +178,7 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -190,7 +186,7 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -199,14 +195,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -218,14 +214,14 @@
     </font>
     <font>
       <sz val="14"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color rgb="FF0070C0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -233,7 +229,7 @@
       <u/>
       <sz val="14"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -241,13 +237,13 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -255,7 +251,7 @@
       <u/>
       <sz val="14"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -264,12 +260,12 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -280,16 +276,6 @@
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="11"/>
       </patternFill>
     </fill>
   </fills>
@@ -306,7 +292,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -337,20 +323,11 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -670,23 +647,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FF288A0-DB40-4E38-9AAF-ADDED2880E84}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="10" width="20.21875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="10" width="32.88671875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="10" width="38.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="10" width="18.5546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="10" width="20.44140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="10" width="17.33203125" collapsed="true"/>
-    <col min="7" max="8" style="10" width="8.88671875" collapsed="true"/>
-    <col min="9" max="16384" style="1" width="8.88671875" collapsed="true"/>
+    <col min="1" max="1" width="20.5" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.296875" style="10" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="35.19921875" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.5" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.5" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.796875" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="8.8984375" style="10" collapsed="1"/>
+    <col min="9" max="16384" width="8.8984375" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>11</v>
       </c>
@@ -706,33 +683,31 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>28</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="14"/>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>37</v>
+        <v>30</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>33</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
@@ -754,29 +729,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6E2E380-41FF-438A-822D-1CBE2A443631}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.21875" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="18.19921875" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="15.88671875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="27.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="21.44140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="21.88671875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="10.44140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="12.109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="9.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="10.5546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="14.44140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="24.5546875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="4.77734375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="15.44140625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="8.0" collapsed="true"/>
-    <col min="14" max="16384" style="2" width="18.21875" collapsed="true"/>
+    <col min="1" max="1" width="15.8984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.69921875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.3984375" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.8984375" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.3984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.09765625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.59765625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.3984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="24.59765625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="4.796875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.3984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="8" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="16384" width="18.19921875" style="2" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>11</v>
       </c>
@@ -817,15 +792,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>4</v>
@@ -837,7 +812,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="3">
-        <v>870000</v>
+        <v>81000</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>2</v>
@@ -852,21 +827,21 @@
         <v>9</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>6</v>
@@ -875,7 +850,7 @@
         <v>5</v>
       </c>
       <c r="G3" s="3">
-        <v>920000</v>
+        <v>92000</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>2</v>
@@ -890,18 +865,18 @@
         <v>30</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>6</v>
@@ -913,7 +888,7 @@
         <v>5</v>
       </c>
       <c r="G4" s="3">
-        <v>920000</v>
+        <v>92000</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>2</v>
@@ -928,7 +903,7 @@
         <v>10</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>